<commit_message>
modified:   README.md 	modified:   cls/KintoneRest.cls 	modified:   "sample/\343\202\265\343\203\263\343\203\227\343\203\253.xlsm" 	modified:   "sample/\344\273\225\346\247\230\350\252\254\346\230\216\346\233\270.xlsx"
</commit_message>
<xml_diff>
--- a/sample/仕様説明書.xlsx
+++ b/sample/仕様説明書.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8205" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13880" windowHeight="6710"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="2" r:id="rId1"/>
     <sheet name="マニュアル" sheetId="3" r:id="rId2"/>
+    <sheet name="拡張" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="322">
   <si>
     <t>サブテーブルの更新も行える事も挙げておきます。</t>
     <rPh sb="7" eb="9">
@@ -3112,12 +3113,1339 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>( appId as Variant) As Dictionary</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GetFormLayout</t>
+  </si>
+  <si>
+    <t>(appId As Variant) As Dictionary</t>
+  </si>
+  <si>
+    <t>(appId As Variant) As Dictionary</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GetAppViews</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GetAppFormInfo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーション情報関連</t>
+    <rPh sb="8" eb="10">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>カンレン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(name As String) As Dictionar</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CreateNewApp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GetAppSettings</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UpdateNewAppSettings</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>■ 拡張機能</t>
+    <rPh sb="2" eb="4">
+      <t>カクチョウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>キノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>本機能はアプリケーション更新用に作成したもので、単純に API を実行するだけのものが殆どです。</t>
+    <rPh sb="0" eb="1">
+      <t>ホン</t>
+    </rPh>
+    <rPh sb="1" eb="3">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ヨウ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>サクセイ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>タン</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>ホトン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻り値の Dictionary オブジェクトの加工やAPIの呼び出し順序を自分でコントロールする必要があります。</t>
+    <rPh sb="0" eb="1">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>カコウ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>ジュンジョ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ジブン</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>対応メソッド：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/k/v1/app/settings.json</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーションの設定情報を取得します。</t>
+    <rPh sb="9" eb="11">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>取得したいアプリケーションIDを指定します。</t>
+    <rPh sb="0" eb="2">
+      <t>シュトク</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーションのフォームのフィールド情報を取得します。</t>
+    <rPh sb="19" eb="21">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>対応メソッド：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/k/v1/app/form/fields.json</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※標準のアプリケーション共通項目も取得されます。</t>
+    <rPh sb="1" eb="3">
+      <t>ヒョウジュン</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>情報には主に、フィールドの型や属性が含まれます。</t>
+    <rPh sb="0" eb="2">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>オモ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>フク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>フォームのレイアウト情報(表示位置や幅等)を取得します。</t>
+    <rPh sb="10" eb="12">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ハバ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>トウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>対応メソッド：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/k/v1/app/form/layout.json</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GetAppProcess</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーションのプロセス情報を取得します。</t>
+    <rPh sb="13" eb="15">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>対応メソッド：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/k/v1/app/process.json</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーションのビュー情報を取得します。</t>
+    <rPh sb="12" eb="14">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>対応メソッド：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>GET</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/k/v1/app/form/views.json</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>新規アプリケーションを作成します。</t>
+    <rPh sb="0" eb="2">
+      <t>シンキ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>作成するアプリの名前を指定します。</t>
+    <rPh sb="0" eb="2">
+      <t>サクセイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>成功すると戻り値には、以下の API のJSON文字列をパースしたオブジェクトが返ります。</t>
+    <rPh sb="0" eb="2">
+      <t>セイコウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="24" eb="27">
+      <t>モジレツ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>対応メソッド：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>POST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/k/v1/preview/app.json</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>デプロイが必要です。</t>
+    <rPh sb="5" eb="7">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>戻り値の重要な項目として、"app"に新規に作成されたアプリIDが格納されます。</t>
+    <rPh sb="0" eb="1">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ジュウヨウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>シンキ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>サクセイ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>カクノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>この状態ではアプリは管理画面で参照は出来ますがアプリとしては利用できません。</t>
+    <rPh sb="2" eb="4">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>カンリ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>デキ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>リヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>( appSettings as Dictionary ) As Variant</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーションの設定情報を更新します。</t>
+    <rPh sb="9" eb="11">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>引数のオブジェクトには以下の API で利用する項目が含まれている必要があります。</t>
+    <rPh sb="0" eb="2">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>従前の情報はGetAppSettingsで取得できます。</t>
+    <rPh sb="0" eb="2">
+      <t>ジュウゼン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>対応メソッド：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>PUT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/k/v1/preview/app/settings.json</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ただし、アプリケーションIDが含まれていないので、付加する必要があります。</t>
+    <rPh sb="15" eb="16">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AddNewAppFormFields</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>( appForm as Dictionary ) As Variant</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>正常に終了した場合、戻り値にはリビジョン番号が返ります。</t>
+    <rPh sb="0" eb="2">
+      <t>セイジョウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>シュウリョウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>チ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>従前の情報はGetAppFormInfoで取得できます。</t>
+    <rPh sb="0" eb="2">
+      <t>ジュウゼン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>また、アプリ共通項目は除く必要があります。</t>
+    <rPh sb="6" eb="8">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ノゾ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UpdateNewAppLayout</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>( appLayout as Dictionary ) As Variant</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーションのフォームの項目を設定します。</t>
+    <rPh sb="14" eb="16">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>対応メソッド：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>POST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/k/v1/preview/app/form/fields.json</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーションのレイアウト情報を更新します。</t>
+    <rPh sb="14" eb="16">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>対応メソッド：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>PUT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/k/v1/preview/app/form/layout.json</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>従前の情報はGetAppLayoutで取得できます。</t>
+    <rPh sb="0" eb="2">
+      <t>ジュウゼン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UpdateNewAppProcess</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>( appProcess as Dictionary ) As Variant</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーションのプロセス情報を更新します。</t>
+    <rPh sb="13" eb="15">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>対応メソッド：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>PUT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/k/v1/preview/app/process.json</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UpdateNewAppViews</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>( appViews as Dictionary ) As Variant</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>アプリケーションのビュー情報を更新します。</t>
+    <rPh sb="12" eb="14">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>コウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>対応メソッド：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>　</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>PUT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>/k/v1/preview/app/views.json</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>従前の情報はGetAppProcessで取得できます。</t>
+    <rPh sb="0" eb="2">
+      <t>ジュウゼン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>従前の情報はGetAppViewsで取得できます。</t>
+    <rPh sb="0" eb="2">
+      <t>ジュウゼン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>シュトク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DeployPreviewApp</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>( appId As Variant) As Variant</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>変更中のアプリケーションをデプロイします。</t>
+    <rPh sb="0" eb="3">
+      <t>ヘンコウチュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>一つのまとまった機能（例えば、「アプリケーションのコピー」）として使うには、</t>
+    <rPh sb="0" eb="1">
+      <t>１</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>タト</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>その為、各 API がどのようなオブジェクトを返すかを理解している必要があります。</t>
+    <rPh sb="2" eb="3">
+      <t>タメ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>カエ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>リカイ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>リビジョンを指定した場合は現在のリビジョンと一致する必要があります。</t>
+    <rPh sb="6" eb="8">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>イッチ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3202,6 +4530,19 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3225,7 +4566,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3248,6 +4589,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3533,123 +4880,123 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="16" width="4" customWidth="1"/>
-    <col min="17" max="26" width="3.875" customWidth="1"/>
-    <col min="27" max="30" width="3.375" customWidth="1"/>
+    <col min="17" max="26" width="3.83203125" customWidth="1"/>
+    <col min="27" max="30" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="29">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3">
       <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" s="2" customFormat="1" ht="15">
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" s="2" customFormat="1" ht="15">
       <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" s="2" customFormat="1" ht="15">
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" s="2" customFormat="1" ht="15">
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" s="2" customFormat="1" ht="15">
       <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" s="2" customFormat="1" ht="15">
       <c r="C14" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" s="2" customFormat="1" ht="15">
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" s="2" customFormat="1" ht="15">
       <c r="C16" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:3" s="2" customFormat="1" ht="15">
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:3" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:3" s="2" customFormat="1" ht="15">
       <c r="C18" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:3">
       <c r="B20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:3">
       <c r="B21" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:3">
       <c r="B23" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:3">
       <c r="B24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:3">
       <c r="B25" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:3">
       <c r="B26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:3">
       <c r="B28" t="s">
         <v>4</v>
       </c>
@@ -3666,11 +5013,11 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B2:W265"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M236" sqref="M236"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A173" sqref="A173:Z173"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="21" width="3.5" customWidth="1"/>
     <col min="22" max="23" width="4" customWidth="1"/>
@@ -3679,32 +5026,32 @@
     <col min="34" max="39" width="3.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:4" s="3" customFormat="1" ht="22.5">
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:4" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:4" s="4" customFormat="1" ht="20">
       <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:4">
       <c r="C9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:4">
       <c r="C11" t="s">
         <v>27</v>
       </c>
@@ -3712,68 +5059,68 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:4">
       <c r="D12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="2:4" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:4" s="4" customFormat="1" ht="20">
       <c r="B14" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="2:4" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" s="4" customFormat="1" ht="20"/>
+    <row r="16" spans="2:4">
       <c r="C16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:20">
       <c r="C17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:20">
       <c r="C19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="2:20" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:20" s="4" customFormat="1" ht="20">
       <c r="B21" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:20">
       <c r="C23" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:20">
       <c r="C24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:20">
       <c r="C25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:20">
       <c r="C26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:20">
       <c r="C27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:20">
       <c r="C28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:20" ht="20">
       <c r="B30" t="s">
         <v>41</v>
       </c>
@@ -3781,28 +5128,28 @@
         <v>244</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:20" ht="20">
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:20">
       <c r="C32" t="s">
         <v>42</v>
       </c>
       <c r="T32" s="6"/>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:22">
       <c r="C33" t="s">
         <v>43</v>
       </c>
       <c r="T33" s="6"/>
     </row>
-    <row r="35" spans="2:22" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:22" s="4" customFormat="1" ht="20">
       <c r="B35" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="2:22" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.4"/>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:22" s="4" customFormat="1" ht="20"/>
+    <row r="37" spans="2:22">
       <c r="C37" t="s">
         <v>45</v>
       </c>
@@ -3819,12 +5166,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:22">
       <c r="M38" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:22">
       <c r="C40" t="s">
         <v>45</v>
       </c>
@@ -3841,12 +5188,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:22">
       <c r="M41" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:22">
       <c r="C43" t="s">
         <v>54</v>
       </c>
@@ -3860,12 +5207,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:22">
       <c r="M44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="2:22" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:22" s="2" customFormat="1" ht="15">
       <c r="N45" s="2" t="s">
         <v>27</v>
       </c>
@@ -3873,28 +5220,28 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="2:22" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:22" s="2" customFormat="1" ht="15">
       <c r="O46" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="2:22" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:22" s="2" customFormat="1" ht="15">
       <c r="P47" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="2:22" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:22" s="2" customFormat="1" ht="15">
       <c r="P48" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="3:23" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="49" spans="3:23" s="2" customFormat="1" ht="15">
       <c r="O49" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="3:23" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.4"/>
-    <row r="51" spans="3:23" x14ac:dyDescent="0.4">
+    <row r="50" spans="3:23" s="7" customFormat="1" ht="15"/>
+    <row r="51" spans="3:23">
       <c r="C51" t="s">
         <v>54</v>
       </c>
@@ -3911,22 +5258,22 @@
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="3:23" x14ac:dyDescent="0.4">
+    <row r="52" spans="3:23">
       <c r="M52" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="3:23" x14ac:dyDescent="0.4">
+    <row r="53" spans="3:23">
       <c r="M53" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="3:23" x14ac:dyDescent="0.4">
+    <row r="54" spans="3:23">
       <c r="M54" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="3:23" x14ac:dyDescent="0.4">
+    <row r="56" spans="3:23">
       <c r="M56" t="s">
         <v>71</v>
       </c>
@@ -3934,17 +5281,17 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="3:23" x14ac:dyDescent="0.4">
+    <row r="57" spans="3:23">
       <c r="N57" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="3:23" x14ac:dyDescent="0.4">
+    <row r="58" spans="3:23">
       <c r="N58" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="3:23" x14ac:dyDescent="0.4">
+    <row r="60" spans="3:23">
       <c r="C60" t="s">
         <v>75</v>
       </c>
@@ -3958,22 +5305,22 @@
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="3:23" x14ac:dyDescent="0.4">
+    <row r="61" spans="3:23">
       <c r="M61" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="3:23" x14ac:dyDescent="0.4">
+    <row r="62" spans="3:23">
       <c r="M62" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="3:23" x14ac:dyDescent="0.4">
+    <row r="63" spans="3:23">
       <c r="M63" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="64" spans="3:23" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="64" spans="3:23" s="2" customFormat="1" ht="15">
       <c r="N64" s="2" t="s">
         <v>27</v>
       </c>
@@ -3981,17 +5328,17 @@
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="2:20" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:20" s="2" customFormat="1" ht="15">
       <c r="P65" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="66" spans="2:20" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:20" s="2" customFormat="1" ht="15">
       <c r="O66" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:20">
       <c r="C68" t="s">
         <v>75</v>
       </c>
@@ -4005,22 +5352,22 @@
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:20">
       <c r="M69" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:20">
       <c r="M70" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:20">
       <c r="M71" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="2:20" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:20" s="2" customFormat="1" ht="15">
       <c r="N72" s="2" t="s">
         <v>27</v>
       </c>
@@ -4028,27 +5375,27 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="2:20" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:20" s="2" customFormat="1" ht="15">
       <c r="P73" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="2:20" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:20" s="2" customFormat="1" ht="15">
       <c r="O74" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="2:20" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="76" spans="2:20" s="4" customFormat="1" ht="20">
       <c r="B76" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="78" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="78" spans="2:20">
       <c r="C78" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="80" spans="2:20" x14ac:dyDescent="0.4">
+    <row r="80" spans="2:20">
       <c r="C80" t="s">
         <v>75</v>
       </c>
@@ -4062,17 +5409,17 @@
         <v>96</v>
       </c>
     </row>
-    <row r="81" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="81" spans="3:20">
       <c r="M81" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="82" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="82" spans="3:20">
       <c r="M82" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="84" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="84" spans="3:20">
       <c r="C84" t="s">
         <v>75</v>
       </c>
@@ -4086,17 +5433,17 @@
         <v>96</v>
       </c>
     </row>
-    <row r="85" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="85" spans="3:20">
       <c r="M85" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="86" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="86" spans="3:20">
       <c r="M86" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="88" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="88" spans="3:20">
       <c r="C88" t="s">
         <v>75</v>
       </c>
@@ -4107,37 +5454,37 @@
         <v>104</v>
       </c>
     </row>
-    <row r="89" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="89" spans="3:20">
       <c r="M89" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="90" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="90" spans="3:20">
       <c r="M90" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="91" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="91" spans="3:20">
       <c r="M91" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="92" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="92" spans="3:20">
       <c r="M92" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="93" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="93" spans="3:20">
       <c r="M93" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="94" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="94" spans="3:20">
       <c r="M94" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="96" spans="3:20" x14ac:dyDescent="0.4">
+    <row r="96" spans="3:20">
       <c r="C96" t="s">
         <v>75</v>
       </c>
@@ -4148,25 +5495,25 @@
         <v>112</v>
       </c>
     </row>
-    <row r="97" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="97" spans="3:13">
       <c r="M97" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="98" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="98" spans="3:13">
       <c r="M98" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="99" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="99" spans="3:13">
       <c r="M99" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="100" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="100" spans="3:13">
       <c r="M100" s="5"/>
     </row>
-    <row r="101" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="101" spans="3:13">
       <c r="C101" t="s">
         <v>75</v>
       </c>
@@ -4177,42 +5524,42 @@
         <v>117</v>
       </c>
     </row>
-    <row r="102" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="102" spans="3:13">
       <c r="M102" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="103" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="103" spans="3:13">
       <c r="M103" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="104" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="104" spans="3:13">
       <c r="M104" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="105" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="105" spans="3:13">
       <c r="M105" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="106" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="106" spans="3:13">
       <c r="M106" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="107" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="107" spans="3:13">
       <c r="M107" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="108" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="108" spans="3:13">
       <c r="M108" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="110" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="110" spans="3:13">
       <c r="C110" t="s">
         <v>75</v>
       </c>
@@ -4223,22 +5570,22 @@
         <v>126</v>
       </c>
     </row>
-    <row r="111" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="111" spans="3:13">
       <c r="M111" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="112" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="112" spans="3:13">
       <c r="M112" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="113" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="113" spans="3:13">
       <c r="M113" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="115" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="115" spans="3:13">
       <c r="C115" t="s">
         <v>75</v>
       </c>
@@ -4249,22 +5596,22 @@
         <v>126</v>
       </c>
     </row>
-    <row r="116" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="116" spans="3:13">
       <c r="M116" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="117" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="117" spans="3:13">
       <c r="M117" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="118" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="118" spans="3:13">
       <c r="M118" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="121" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="121" spans="3:13">
       <c r="C121" t="s">
         <v>75</v>
       </c>
@@ -4275,22 +5622,22 @@
         <v>135</v>
       </c>
     </row>
-    <row r="122" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="122" spans="3:13">
       <c r="M122" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="123" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="123" spans="3:13">
       <c r="M123" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="124" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="124" spans="3:13">
       <c r="M124" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="126" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="126" spans="3:13">
       <c r="C126" t="s">
         <v>54</v>
       </c>
@@ -4301,32 +5648,32 @@
         <v>140</v>
       </c>
     </row>
-    <row r="127" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="127" spans="3:13">
       <c r="M127" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="128" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="128" spans="3:13">
       <c r="M128" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="129" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="129" spans="3:13">
       <c r="M129" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="130" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="130" spans="3:13">
       <c r="M130" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="131" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="131" spans="3:13">
       <c r="M131" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="134" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="134" spans="3:13">
       <c r="C134" t="s">
         <v>75</v>
       </c>
@@ -4337,22 +5684,22 @@
         <v>135</v>
       </c>
     </row>
-    <row r="135" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="135" spans="3:13">
       <c r="M135" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="136" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="136" spans="3:13">
       <c r="M136" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="137" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="137" spans="3:13">
       <c r="M137" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="139" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="139" spans="3:13">
       <c r="C139" t="s">
         <v>75</v>
       </c>
@@ -4363,37 +5710,37 @@
         <v>148</v>
       </c>
     </row>
-    <row r="140" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="140" spans="3:13">
       <c r="M140" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="141" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="141" spans="3:13">
       <c r="M141" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="142" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="142" spans="3:13">
       <c r="M142" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="143" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="143" spans="3:13">
       <c r="M143" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="144" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="144" spans="3:13">
       <c r="M144" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="146" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="146" spans="3:13">
       <c r="C146" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="148" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="148" spans="3:13">
       <c r="C148" t="s">
         <v>75</v>
       </c>
@@ -4404,22 +5751,22 @@
         <v>156</v>
       </c>
     </row>
-    <row r="149" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="149" spans="3:13">
       <c r="M149" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="150" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="150" spans="3:13">
       <c r="M150" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="151" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="151" spans="3:13">
       <c r="M151" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="153" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="153" spans="3:13">
       <c r="C153" t="s">
         <v>75</v>
       </c>
@@ -4430,25 +5777,25 @@
         <v>161</v>
       </c>
     </row>
-    <row r="154" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="154" spans="3:13">
       <c r="M154" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="155" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="155" spans="3:13">
       <c r="M155" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="156" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="156" spans="3:13">
       <c r="M156" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="157" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="157" spans="3:13">
       <c r="M157" s="5"/>
     </row>
-    <row r="158" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="158" spans="3:13">
       <c r="C158" t="s">
         <v>75</v>
       </c>
@@ -4459,25 +5806,25 @@
         <v>161</v>
       </c>
     </row>
-    <row r="159" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="159" spans="3:13">
       <c r="M159" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="160" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="160" spans="3:13">
       <c r="M160" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="161" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="161" spans="2:13">
       <c r="M161" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="162" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="162" spans="2:13">
       <c r="M162" s="5"/>
     </row>
-    <row r="163" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="163" spans="2:13">
       <c r="C163" t="s">
         <v>75</v>
       </c>
@@ -4489,32 +5836,32 @@
       </c>
       <c r="M163" s="5"/>
     </row>
-    <row r="164" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="164" spans="2:13">
       <c r="M164" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="165" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="165" spans="2:13">
       <c r="M165" s="5" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="166" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="166" spans="2:13">
       <c r="M166" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="168" spans="2:13" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="168" spans="2:13" s="4" customFormat="1" ht="20">
       <c r="B168" s="4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="170" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="170" spans="2:13">
       <c r="C170" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="172" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="172" spans="2:13">
       <c r="C172" t="s">
         <v>75</v>
       </c>
@@ -4525,27 +5872,27 @@
         <v>175</v>
       </c>
     </row>
-    <row r="173" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="173" spans="2:13">
       <c r="M173" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="174" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="174" spans="2:13">
       <c r="M174" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="175" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="175" spans="2:13">
       <c r="M175" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="176" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="176" spans="2:13">
       <c r="M176" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="178" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="178" spans="3:13">
       <c r="C178" t="s">
         <v>75</v>
       </c>
@@ -4556,37 +5903,37 @@
         <v>181</v>
       </c>
     </row>
-    <row r="179" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="179" spans="3:13">
       <c r="M179" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="180" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="180" spans="3:13">
       <c r="M180" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="181" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="181" spans="3:13">
       <c r="M181" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="183" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="183" spans="3:13">
       <c r="C183" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="185" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="185" spans="3:13">
       <c r="D185" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="186" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="186" spans="3:13">
       <c r="D186" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="188" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="188" spans="3:13">
       <c r="C188" t="s">
         <v>75</v>
       </c>
@@ -4597,22 +5944,22 @@
         <v>189</v>
       </c>
     </row>
-    <row r="189" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="189" spans="3:13">
       <c r="M189" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="190" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="190" spans="3:13">
       <c r="M190" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="191" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="191" spans="3:13">
       <c r="M191" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="193" spans="2:13">
       <c r="C193" t="s">
         <v>75</v>
       </c>
@@ -4623,32 +5970,32 @@
         <v>193</v>
       </c>
     </row>
-    <row r="194" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="194" spans="2:13">
       <c r="M194" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="195" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="195" spans="2:13">
       <c r="M195" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="196" spans="2:13">
       <c r="M196" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="197" spans="2:13">
       <c r="M197" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="198" spans="2:13">
       <c r="M198" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="200" spans="2:13">
       <c r="C200" t="s">
         <v>75</v>
       </c>
@@ -4659,133 +6006,133 @@
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="201" spans="2:13">
       <c r="M201" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="202" spans="2:13">
       <c r="M202" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="203" spans="2:13">
       <c r="M203" s="5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="204" spans="2:13">
       <c r="M204" s="5" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="205" spans="2:13">
       <c r="M205" s="5"/>
     </row>
-    <row r="207" spans="2:13" s="4" customFormat="1" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="207" spans="2:13" s="4" customFormat="1" ht="20">
       <c r="B207" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="209" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="209" spans="3:3">
       <c r="C209" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="211" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="211" spans="3:3">
       <c r="C211" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="213" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="213" spans="3:3">
       <c r="C213" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="215" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="215" spans="3:3">
       <c r="C215" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="216" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="216" spans="3:3">
       <c r="C216" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="217" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="217" spans="3:3">
       <c r="C217" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="218" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="218" spans="3:3">
       <c r="C218" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="219" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="219" spans="3:3">
       <c r="C219" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="220" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="220" spans="3:3">
       <c r="C220" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="221" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="221" spans="3:3">
       <c r="C221" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="222" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="222" spans="3:3">
       <c r="C222" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="223" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="223" spans="3:3">
       <c r="C223" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="224" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="224" spans="3:3">
       <c r="C224" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="226" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="226" spans="2:13">
       <c r="C226" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="227" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="227" spans="2:13">
       <c r="D227" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="228" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="228" spans="2:13">
       <c r="D228" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="229" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="229" spans="2:13">
       <c r="D229" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="231" spans="2:13" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="231" spans="2:13" ht="20">
       <c r="B231" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="232" spans="2:13" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="232" spans="2:13" ht="20">
       <c r="B232" s="4"/>
     </row>
-    <row r="233" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="233" spans="2:13">
       <c r="C233" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="235" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="235" spans="2:13">
       <c r="C235" t="s">
         <v>75</v>
       </c>
@@ -4796,7 +6143,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="236" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="236" spans="2:13">
       <c r="C236" t="s">
         <v>75</v>
       </c>
@@ -4807,7 +6154,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="237" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="237" spans="2:13">
       <c r="C237" t="s">
         <v>75</v>
       </c>
@@ -4818,7 +6165,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="238" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="238" spans="2:13">
       <c r="C238" t="s">
         <v>75</v>
       </c>
@@ -4829,42 +6176,42 @@
         <v>229</v>
       </c>
     </row>
-    <row r="240" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="240" spans="2:13">
       <c r="C240" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="241" spans="2:4">
       <c r="C241" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="242" spans="2:4">
       <c r="C242" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="243" spans="2:4">
       <c r="C243" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="244" spans="2:4">
       <c r="C244" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="246" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="246" spans="2:4" ht="20">
       <c r="B246" s="4" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="248" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="248" spans="2:4">
       <c r="C248" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="250" spans="2:4">
       <c r="C250" t="s">
         <v>75</v>
       </c>
@@ -4872,7 +6219,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="251" spans="2:4">
       <c r="C251" t="s">
         <v>75</v>
       </c>
@@ -4880,7 +6227,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="252" spans="2:4">
       <c r="C252" t="s">
         <v>239</v>
       </c>
@@ -4888,7 +6235,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="253" spans="2:4">
       <c r="C253" t="s">
         <v>239</v>
       </c>
@@ -4896,7 +6243,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="254" spans="2:4">
       <c r="C254" t="s">
         <v>75</v>
       </c>
@@ -4904,36 +6251,570 @@
         <v>242</v>
       </c>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="256" spans="2:4">
       <c r="C256" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="258" spans="2:3" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="258" spans="2:3" ht="20">
       <c r="B258" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="260" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="260" spans="2:3">
       <c r="C260" s="5" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="261" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="261" spans="2:3">
       <c r="C261" s="5" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="262" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="262" spans="2:3">
       <c r="C262" s="5" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="263" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="263" spans="2:3">
       <c r="C263" s="5"/>
     </row>
-    <row r="265" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="265" spans="2:3">
       <c r="C265" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A2:M101"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W101" sqref="W101"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="18" width="3.5" customWidth="1"/>
+    <col min="19" max="28" width="3.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" ht="20">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="C4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="D5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="D6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="D7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="D8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="20">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>262</v>
+      </c>
+      <c r="J12" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="M13" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="M14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="M15" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="M16" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13">
+      <c r="C18" t="s">
+        <v>257</v>
+      </c>
+      <c r="D18" t="s">
+        <v>258</v>
+      </c>
+      <c r="J18" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13">
+      <c r="M19" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13">
+      <c r="M20" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13">
+      <c r="M21" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13">
+      <c r="M22" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13">
+      <c r="M23" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13">
+      <c r="M24" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13">
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
+        <v>252</v>
+      </c>
+      <c r="J26" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13">
+      <c r="M27" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13">
+      <c r="M28" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13">
+      <c r="M29" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13">
+      <c r="M30" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13">
+      <c r="C32" t="s">
+        <v>255</v>
+      </c>
+      <c r="D32" t="s">
+        <v>276</v>
+      </c>
+      <c r="J32" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13">
+      <c r="M33" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13">
+      <c r="M34" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13">
+      <c r="M35" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="36" spans="3:13">
+      <c r="M36" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13">
+      <c r="C38" t="s">
+        <v>255</v>
+      </c>
+      <c r="D38" t="s">
+        <v>256</v>
+      </c>
+      <c r="J38" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="39" spans="3:13">
+      <c r="M39" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="40" spans="3:13">
+      <c r="M40" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="41" spans="3:13">
+      <c r="M41" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="42" spans="3:13">
+      <c r="M42" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13">
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" t="s">
+        <v>261</v>
+      </c>
+      <c r="J44" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="45" spans="3:13">
+      <c r="M45" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="46" spans="3:13">
+      <c r="M46" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="47" spans="3:13">
+      <c r="M47" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="48" spans="3:13">
+      <c r="M48" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="49" spans="3:13">
+      <c r="M49" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="50" spans="3:13">
+      <c r="M50" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="51" spans="3:13">
+      <c r="M51" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="53" spans="3:13">
+      <c r="C53" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" t="s">
+        <v>263</v>
+      </c>
+      <c r="J53" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="54" spans="3:13">
+      <c r="M54" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="55" spans="3:13">
+      <c r="M55" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="56" spans="3:13">
+      <c r="M56" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="57" spans="3:13">
+      <c r="M57" s="9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="58" spans="3:13">
+      <c r="M58" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="59" spans="3:13">
+      <c r="M59" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="60" spans="3:13">
+      <c r="M60" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="62" spans="3:13">
+      <c r="C62" t="s">
+        <v>45</v>
+      </c>
+      <c r="D62" t="s">
+        <v>294</v>
+      </c>
+      <c r="J62" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="63" spans="3:13">
+      <c r="M63" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="64" spans="3:13">
+      <c r="M64" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="65" spans="3:13">
+      <c r="M65" s="8" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="66" spans="3:13">
+      <c r="M66" s="9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="67" spans="3:13">
+      <c r="M67" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="68" spans="3:13">
+      <c r="M68" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="69" spans="3:13">
+      <c r="M69" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="70" spans="3:13">
+      <c r="M70" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="72" spans="3:13">
+      <c r="C72" t="s">
+        <v>45</v>
+      </c>
+      <c r="D72" t="s">
+        <v>299</v>
+      </c>
+      <c r="J72" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="73" spans="3:13">
+      <c r="M73" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="74" spans="3:13">
+      <c r="M74" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="75" spans="3:13">
+      <c r="M75" s="8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="76" spans="3:13">
+      <c r="M76" s="9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="77" spans="3:13">
+      <c r="M77" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="78" spans="3:13">
+      <c r="M78" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="79" spans="3:13">
+      <c r="M79" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="81" spans="3:13">
+      <c r="C81" t="s">
+        <v>45</v>
+      </c>
+      <c r="D81" t="s">
+        <v>306</v>
+      </c>
+      <c r="J81" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="82" spans="3:13">
+      <c r="M82" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="83" spans="3:13">
+      <c r="M83" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="84" spans="3:13">
+      <c r="M84" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="85" spans="3:13">
+      <c r="M85" s="9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="86" spans="3:13">
+      <c r="M86" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="87" spans="3:13">
+      <c r="M87" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="88" spans="3:13">
+      <c r="M88" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="90" spans="3:13">
+      <c r="C90" t="s">
+        <v>45</v>
+      </c>
+      <c r="D90" t="s">
+        <v>310</v>
+      </c>
+      <c r="J90" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="91" spans="3:13">
+      <c r="M91" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="92" spans="3:13">
+      <c r="M92" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="93" spans="3:13">
+      <c r="M93" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="94" spans="3:13">
+      <c r="M94" s="9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="95" spans="3:13">
+      <c r="M95" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="96" spans="3:13">
+      <c r="M96" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="97" spans="3:13">
+      <c r="M97" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="99" spans="3:13">
+      <c r="C99" t="s">
+        <v>45</v>
+      </c>
+      <c r="D99" t="s">
+        <v>316</v>
+      </c>
+      <c r="J99" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="100" spans="3:13">
+      <c r="M100" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="101" spans="3:13">
+      <c r="M101" s="9" t="s">
+        <v>296</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>